<commit_message>
with 256-levels of grey
</commit_message>
<xml_diff>
--- a/scsi2/scans/Scanner File Size.xlsx
+++ b/scsi2/scans/Scanner File Size.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antoine/Documents/antoine/apple iigs/crossdevtools/source/scsi2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antoine/Documents/antoine/apple iigs/crossdevtools/source/scsi2/scans/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33388224-E115-4D4A-97DF-BE940AD27EC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F79732-4C18-304F-9982-04D4200F574D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{A858CC69-06A7-744D-A325-4FC29BE3E03D}"/>
   </bookViews>
@@ -437,7 +437,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -447,7 +447,7 @@
         <v>13</v>
       </c>
       <c r="B1">
-        <v>8.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -455,7 +455,7 @@
         <v>14</v>
       </c>
       <c r="B2">
-        <v>11</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -472,7 +472,7 @@
       </c>
       <c r="B5">
         <f>B1*B10</f>
-        <v>10200</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -489,7 +489,7 @@
       </c>
       <c r="B8">
         <f>B2*B10</f>
-        <v>13200</v>
+        <v>4200</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -505,7 +505,7 @@
         <v>5</v>
       </c>
       <c r="B12">
-        <v>75</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -513,7 +513,7 @@
         <v>6</v>
       </c>
       <c r="B13">
-        <v>75</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -530,7 +530,7 @@
       </c>
       <c r="B15">
         <f>IF(B12=75,16,IF(B12=150,8,0))</f>
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -539,7 +539,7 @@
       </c>
       <c r="B17">
         <f>B5-B4+B15</f>
-        <v>10216</v>
+        <v>6008</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -548,7 +548,7 @@
       </c>
       <c r="B18">
         <f>B8-B7</f>
-        <v>13200</v>
+        <v>4200</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -557,7 +557,7 @@
       </c>
       <c r="B20">
         <f>ROUNDDOWN(((B17*B12)/B10)*(B14/8),0)</f>
-        <v>638</v>
+        <v>751</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -566,7 +566,7 @@
       </c>
       <c r="B21">
         <f>(B18*B13)/B10</f>
-        <v>825</v>
+        <v>525</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -575,7 +575,7 @@
       </c>
       <c r="B22">
         <f>B20*B21</f>
-        <v>526350</v>
+        <v>394275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>